<commit_message>
Added pac diagram data and script for Ext Figure 5a plot. Minor updates to PAC_Diagrams_7a.ipynb. Added spreadsheets for Extended Data Figure 7 alpha power.
</commit_message>
<xml_diff>
--- a/Extended Data Figure 7/alphaPowerLeftSTN_Ext7a.xlsx
+++ b/Extended Data Figure 7/alphaPowerLeftSTN_Ext7a.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slack\Github\nature-bme-2024-dcs-pd\Extended Data Figure 7\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB8157E-67FA-4803-AAED-53EE536867DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="3984" yWindow="2484" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,15 +24,33 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>OFF Pre-op</t>
+  </si>
+  <si>
+    <t>OFF Post-op</t>
+  </si>
+  <si>
+    <t>DCS-P2</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -49,8 +73,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +355,132 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="3" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>0.13941390229079501</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.20930321573712601</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.196557193564451</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>8.5462824872357901E-2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.146737267056747</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.14762375977915301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>7.2806262996169893E-2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.12784250595379601</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.179867071228175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>8.7909183305049196E-2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.120380478682331</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.13952919185812801</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>7.7039934990282402E-2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.16514477906925101</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.13103633343806301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>0.123901976163654</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.17174324658212001</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.11155736866136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1">
+        <v>7.3145008425080996E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1">
+        <v>9.8551642935804998E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1">
+        <v>0.10279716489537701</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1">
+        <v>8.3531123792990297E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1">
+        <v>0.110125720772694</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1">
+        <v>0.19008619760360801</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>